<commit_message>
Updated Readme, cleaned project structure
</commit_message>
<xml_diff>
--- a/Project Gantt Chart.xlsx
+++ b/Project Gantt Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E7BF8D-D7A3-413E-A194-A69D55130415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECDA3F8-9A19-4181-B9EF-C986128A8A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1315,23 +1315,23 @@
     <xf numFmtId="168" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1944,7 +1944,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BP9" sqref="BP9"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1989,107 +1989,107 @@
         <v>2</v>
       </c>
       <c r="B3" s="51"/>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="93">
+      <c r="D3" s="93"/>
+      <c r="E3" s="91">
         <f ca="1">TODAY()</f>
-        <v>45590</v>
-      </c>
-      <c r="F3" s="93"/>
+        <v>45773</v>
+      </c>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="88">
         <f ca="1">I5</f>
-        <v>45586</v>
-      </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="90">
+        <v>45768</v>
+      </c>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f ca="1">P5</f>
-        <v>45593</v>
-      </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="90">
+        <v>45775</v>
+      </c>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f ca="1">W5</f>
-        <v>45600</v>
-      </c>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="90">
+        <v>45782</v>
+      </c>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f ca="1">AD5</f>
-        <v>45607</v>
-      </c>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="90">
+        <v>45789</v>
+      </c>
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f ca="1">AK5</f>
-        <v>45614</v>
-      </c>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="90">
+        <v>45796</v>
+      </c>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f ca="1">AR5</f>
-        <v>45621</v>
-      </c>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="90">
+        <v>45803</v>
+      </c>
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f ca="1">AY5</f>
-        <v>45628</v>
-      </c>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="90">
+        <v>45810</v>
+      </c>
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f ca="1">BF5</f>
-        <v>45635</v>
-      </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="92"/>
+        <v>45817</v>
+      </c>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
@@ -2103,227 +2103,227 @@
       <c r="G5" s="66"/>
       <c r="I5" s="85">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45586</v>
+        <v>45768</v>
       </c>
       <c r="J5" s="86">
         <f ca="1">I5+1</f>
-        <v>45587</v>
+        <v>45769</v>
       </c>
       <c r="K5" s="86">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45588</v>
+        <v>45770</v>
       </c>
       <c r="L5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45589</v>
+        <v>45771</v>
       </c>
       <c r="M5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45590</v>
+        <v>45772</v>
       </c>
       <c r="N5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45591</v>
+        <v>45773</v>
       </c>
       <c r="O5" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>45592</v>
+        <v>45774</v>
       </c>
       <c r="P5" s="85">
         <f ca="1">O5+1</f>
-        <v>45593</v>
+        <v>45775</v>
       </c>
       <c r="Q5" s="86">
         <f ca="1">P5+1</f>
-        <v>45594</v>
+        <v>45776</v>
       </c>
       <c r="R5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45595</v>
+        <v>45777</v>
       </c>
       <c r="S5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45596</v>
+        <v>45778</v>
       </c>
       <c r="T5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45597</v>
+        <v>45779</v>
       </c>
       <c r="U5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45598</v>
+        <v>45780</v>
       </c>
       <c r="V5" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>45599</v>
+        <v>45781</v>
       </c>
       <c r="W5" s="85">
         <f ca="1">V5+1</f>
-        <v>45600</v>
+        <v>45782</v>
       </c>
       <c r="X5" s="86">
         <f ca="1">W5+1</f>
-        <v>45601</v>
+        <v>45783</v>
       </c>
       <c r="Y5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45602</v>
+        <v>45784</v>
       </c>
       <c r="Z5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45603</v>
+        <v>45785</v>
       </c>
       <c r="AA5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45604</v>
+        <v>45786</v>
       </c>
       <c r="AB5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45605</v>
+        <v>45787</v>
       </c>
       <c r="AC5" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>45606</v>
+        <v>45788</v>
       </c>
       <c r="AD5" s="85">
         <f ca="1">AC5+1</f>
-        <v>45607</v>
+        <v>45789</v>
       </c>
       <c r="AE5" s="86">
         <f ca="1">AD5+1</f>
-        <v>45608</v>
+        <v>45790</v>
       </c>
       <c r="AF5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45609</v>
+        <v>45791</v>
       </c>
       <c r="AG5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45610</v>
+        <v>45792</v>
       </c>
       <c r="AH5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45611</v>
+        <v>45793</v>
       </c>
       <c r="AI5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45612</v>
+        <v>45794</v>
       </c>
       <c r="AJ5" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>45613</v>
+        <v>45795</v>
       </c>
       <c r="AK5" s="85">
         <f ca="1">AJ5+1</f>
-        <v>45614</v>
+        <v>45796</v>
       </c>
       <c r="AL5" s="86">
         <f ca="1">AK5+1</f>
-        <v>45615</v>
+        <v>45797</v>
       </c>
       <c r="AM5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45616</v>
+        <v>45798</v>
       </c>
       <c r="AN5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45617</v>
+        <v>45799</v>
       </c>
       <c r="AO5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45618</v>
+        <v>45800</v>
       </c>
       <c r="AP5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45619</v>
+        <v>45801</v>
       </c>
       <c r="AQ5" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>45620</v>
+        <v>45802</v>
       </c>
       <c r="AR5" s="85">
         <f ca="1">AQ5+1</f>
-        <v>45621</v>
+        <v>45803</v>
       </c>
       <c r="AS5" s="86">
         <f ca="1">AR5+1</f>
-        <v>45622</v>
+        <v>45804</v>
       </c>
       <c r="AT5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45623</v>
+        <v>45805</v>
       </c>
       <c r="AU5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45624</v>
+        <v>45806</v>
       </c>
       <c r="AV5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45625</v>
+        <v>45807</v>
       </c>
       <c r="AW5" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>45626</v>
+        <v>45808</v>
       </c>
       <c r="AX5" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>45627</v>
+        <v>45809</v>
       </c>
       <c r="AY5" s="85">
         <f ca="1">AX5+1</f>
-        <v>45628</v>
+        <v>45810</v>
       </c>
       <c r="AZ5" s="86">
         <f ca="1">AY5+1</f>
-        <v>45629</v>
+        <v>45811</v>
       </c>
       <c r="BA5" s="86">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45630</v>
+        <v>45812</v>
       </c>
       <c r="BB5" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>45631</v>
+        <v>45813</v>
       </c>
       <c r="BC5" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>45632</v>
+        <v>45814</v>
       </c>
       <c r="BD5" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>45633</v>
+        <v>45815</v>
       </c>
       <c r="BE5" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>45634</v>
+        <v>45816</v>
       </c>
       <c r="BF5" s="85">
         <f ca="1">BE5+1</f>
-        <v>45635</v>
+        <v>45817</v>
       </c>
       <c r="BG5" s="86">
         <f ca="1">BF5+1</f>
-        <v>45636</v>
+        <v>45818</v>
       </c>
       <c r="BH5" s="86">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45637</v>
+        <v>45819</v>
       </c>
       <c r="BI5" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>45638</v>
+        <v>45820</v>
       </c>
       <c r="BJ5" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>45639</v>
+        <v>45821</v>
       </c>
       <c r="BK5" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>45640</v>
+        <v>45822</v>
       </c>
       <c r="BL5" s="87">
         <f t="shared" ca="1" si="2"/>
-        <v>45641</v>
+        <v>45823</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2725,15 +2725,15 @@
         <v>48</v>
       </c>
       <c r="D9" s="17">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="E9" s="72">
         <f ca="1">Project_Start</f>
-        <v>45590</v>
+        <v>45773</v>
       </c>
       <c r="F9" s="72">
         <f ca="1">E9+7</f>
-        <v>45597</v>
+        <v>45780</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14">
@@ -2808,15 +2808,15 @@
         <v>49</v>
       </c>
       <c r="D10" s="17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="72">
         <f ca="1">F9</f>
-        <v>45597</v>
+        <v>45780</v>
       </c>
       <c r="F10" s="72">
         <f ca="1">E10+2</f>
-        <v>45599</v>
+        <v>45782</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14">
@@ -2889,15 +2889,15 @@
         <v>51</v>
       </c>
       <c r="D11" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="72">
         <f ca="1">F10</f>
-        <v>45599</v>
+        <v>45782</v>
       </c>
       <c r="F11" s="72">
         <f ca="1">E11+4</f>
-        <v>45603</v>
+        <v>45786</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14">
@@ -2970,11 +2970,11 @@
         <v>53</v>
       </c>
       <c r="D12" s="17">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E12" s="72">
         <f ca="1">E9</f>
-        <v>45590</v>
+        <v>45773</v>
       </c>
       <c r="F12" s="72">
         <v>45714</v>
@@ -2982,7 +2982,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>125</v>
+        <v>-58</v>
       </c>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
@@ -3049,10 +3049,12 @@
       <c r="C13" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="17">
+        <v>0.75</v>
+      </c>
       <c r="E13" s="72">
         <f ca="1">E9</f>
-        <v>45590</v>
+        <v>45773</v>
       </c>
       <c r="F13" s="72">
         <v>45733</v>
@@ -3060,7 +3062,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14">
         <f t="shared" ca="1" si="6"/>
-        <v>144</v>
+        <v>-39</v>
       </c>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
@@ -3201,15 +3203,15 @@
         <v>56</v>
       </c>
       <c r="D15" s="20">
-        <v>0.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E15" s="75">
         <f ca="1">E9</f>
-        <v>45590</v>
+        <v>45773</v>
       </c>
       <c r="F15" s="75">
         <f ca="1">E15+21</f>
-        <v>45611</v>
+        <v>45794</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14">
@@ -3286,11 +3288,11 @@
       </c>
       <c r="E16" s="75">
         <f ca="1">E15+2</f>
-        <v>45592</v>
+        <v>45775</v>
       </c>
       <c r="F16" s="75">
         <f ca="1">E16+25</f>
-        <v>45617</v>
+        <v>45800</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14">
@@ -3365,11 +3367,11 @@
       <c r="D17" s="20"/>
       <c r="E17" s="75">
         <f ca="1">F16</f>
-        <v>45617</v>
+        <v>45800</v>
       </c>
       <c r="F17" s="75">
         <f ca="1">E17+7</f>
-        <v>45624</v>
+        <v>45807</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14">
@@ -3444,11 +3446,11 @@
       <c r="D18" s="20"/>
       <c r="E18" s="75">
         <f ca="1">E17 - 3</f>
-        <v>45614</v>
+        <v>45797</v>
       </c>
       <c r="F18" s="75">
         <f ca="1">E18+15</f>
-        <v>45629</v>
+        <v>45812</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14">
@@ -3523,11 +3525,11 @@
       <c r="D19" s="20"/>
       <c r="E19" s="75">
         <f ca="1">F18</f>
-        <v>45629</v>
+        <v>45812</v>
       </c>
       <c r="F19" s="75">
         <f ca="1">E19+15</f>
-        <v>45644</v>
+        <v>45827</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14">
@@ -3673,11 +3675,11 @@
       <c r="D21" s="23"/>
       <c r="E21" s="78">
         <f ca="1">E9+15</f>
-        <v>45605</v>
+        <v>45788</v>
       </c>
       <c r="F21" s="78">
         <f ca="1">E21+5</f>
-        <v>45610</v>
+        <v>45793</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14">
@@ -3750,11 +3752,11 @@
       <c r="D22" s="23"/>
       <c r="E22" s="78">
         <f ca="1">F21+1</f>
-        <v>45611</v>
+        <v>45794</v>
       </c>
       <c r="F22" s="78">
         <f ca="1">E22+4</f>
-        <v>45615</v>
+        <v>45798</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14">
@@ -3827,11 +3829,11 @@
       <c r="D23" s="23"/>
       <c r="E23" s="78">
         <f ca="1">E22+5</f>
-        <v>45616</v>
+        <v>45799</v>
       </c>
       <c r="F23" s="78">
         <f ca="1">E23+5</f>
-        <v>45621</v>
+        <v>45804</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14">
@@ -3904,11 +3906,11 @@
       <c r="D24" s="23"/>
       <c r="E24" s="78">
         <f ca="1">F23+1</f>
-        <v>45622</v>
+        <v>45805</v>
       </c>
       <c r="F24" s="78">
         <f ca="1">E24+4</f>
-        <v>45626</v>
+        <v>45809</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14">
@@ -3981,11 +3983,11 @@
       <c r="D25" s="23"/>
       <c r="E25" s="78">
         <f ca="1">E23</f>
-        <v>45616</v>
+        <v>45799</v>
       </c>
       <c r="F25" s="78">
         <f ca="1">E25+4</f>
-        <v>45620</v>
+        <v>45803</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14">
@@ -4653,17 +4655,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">
@@ -4834,23 +4836,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5142,22 +5133,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5184,9 +5182,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>